<commit_message>
Fix some figures and plot some first picks
</commit_message>
<xml_diff>
--- a/fallClean/Figures/first_picks_fall_graphs.xlsx
+++ b/fallClean/Figures/first_picks_fall_graphs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabby/Desktop/dragraceAnalysis-master/fallClean/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{202F4A48-E24F-1440-B7F5-2FEA446DEFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962FCE6F-0E34-244E-A0DE-9462C8416646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="460" windowWidth="24160" windowHeight="16300" xr2:uid="{A4149AAE-36FF-8D4D-9AF5-038401B5F3A1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24160" windowHeight="16280" xr2:uid="{A4149AAE-36FF-8D4D-9AF5-038401B5F3A1}"/>
   </bookViews>
   <sheets>
     <sheet name="first_picks_fall" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2267,7 +2267,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>first_picks_fall!$A$13:$A$16</c:f>
+              <c:f>first_picks_fall!$A$20:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2288,7 +2288,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>first_picks_fall!$B$13:$B$16</c:f>
+              <c:f>first_picks_fall!$B$20:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3208,15 +3208,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>572562</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>13884</xdr:rowOff>
+      <xdr:colOff>548823</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>108838</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>104666</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>118140</xdr:rowOff>
+      <xdr:colOff>80927</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>23187</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3541,15 +3541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091E0198-BAE5-1D46-BA78-6F3D9A19ED03}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="107" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>60</v>
       </c>
@@ -3670,8 +3670,11 @@
         <f>AVERAGE(B2:S2)</f>
         <v>722.10578888490522</v>
       </c>
+      <c r="U2">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>330</v>
       </c>
@@ -3733,8 +3736,11 @@
         <f>AVERAGE(B3:S3)</f>
         <v>723.02245085549328</v>
       </c>
+      <c r="U3">
+        <v>330</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>660</v>
       </c>
@@ -3796,8 +3802,11 @@
         <f>AVERAGE(B4:S4)</f>
         <v>795.83339451139761</v>
       </c>
+      <c r="U4">
+        <v>660</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -3859,8 +3868,11 @@
         <f>AVERAGE(B5:S5)</f>
         <v>713.8876812762901</v>
       </c>
+      <c r="U5">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>660</v>
       </c>
@@ -3916,7 +3928,7 @@
         <v>284.33</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>660</v>
       </c>
@@ -3975,73 +3987,207 @@
         <v>282.24</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>325.77</v>
+      </c>
+      <c r="C8">
+        <v>331.69</v>
+      </c>
+      <c r="D8">
+        <v>325.92</v>
+      </c>
+      <c r="E8">
+        <v>168.75</v>
+      </c>
+      <c r="F8">
+        <v>91.99</v>
+      </c>
+      <c r="G8">
+        <v>312.35000000000002</v>
+      </c>
+      <c r="H8">
+        <v>328.14</v>
+      </c>
+      <c r="I8">
+        <v>317.72000000000003</v>
+      </c>
+      <c r="J8">
+        <v>325.14</v>
+      </c>
+      <c r="K8">
+        <v>326.24</v>
+      </c>
+      <c r="M8">
+        <v>328.46</v>
+      </c>
+      <c r="N8">
+        <v>325.92</v>
+      </c>
+      <c r="O8">
+        <v>327.9</v>
+      </c>
+      <c r="P8">
+        <v>190.78</v>
+      </c>
+      <c r="Q8">
+        <v>333.25</v>
+      </c>
+      <c r="R8">
+        <v>330.96</v>
+      </c>
+      <c r="S8">
+        <v>324.58999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>328.06</v>
+      </c>
+      <c r="C9">
+        <v>328.46</v>
+      </c>
+      <c r="D9">
+        <v>329.5</v>
+      </c>
+      <c r="E9">
+        <v>184.19</v>
+      </c>
+      <c r="F9">
+        <v>328.7</v>
+      </c>
+      <c r="G9">
+        <v>323.5</v>
+      </c>
+      <c r="H9">
+        <v>324.83</v>
+      </c>
+      <c r="I9">
+        <v>183.94</v>
+      </c>
+      <c r="J9">
+        <v>325.92</v>
+      </c>
+      <c r="K9">
+        <v>131.79</v>
+      </c>
+      <c r="L9">
+        <v>316.14999999999998</v>
+      </c>
+      <c r="M9">
+        <v>249.53</v>
+      </c>
+      <c r="N9">
+        <v>329.5</v>
+      </c>
+      <c r="O9">
+        <v>321.04000000000002</v>
+      </c>
+      <c r="P9">
+        <v>323.12</v>
+      </c>
+      <c r="Q9">
+        <v>321.81</v>
+      </c>
+      <c r="R9">
+        <v>328.06</v>
+      </c>
+      <c r="S9">
+        <v>332.18000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B17" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>1.3469999999999999E-2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>731.8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>60</v>
       </c>
-      <c r="B13">
-        <f>($A$11*A13) +$A$12</f>
+      <c r="B20">
+        <f>($A$18*A20) +$A$19</f>
         <v>732.60820000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>330</v>
       </c>
-      <c r="B14">
-        <f>($A$11*A14) +$A$12</f>
+      <c r="B21">
+        <f>($A$18*A21) +$A$19</f>
         <v>736.24509999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>660</v>
       </c>
-      <c r="B15">
-        <f>($A$11*A15) +$A$12</f>
+      <c r="B22">
+        <f>($A$18*A22) +$A$19</f>
         <v>740.6902</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>1000</v>
       </c>
-      <c r="B16">
-        <f>($A$11*A16) +$A$12</f>
+      <c r="B23">
+        <f>($A$18*A23) +$A$19</f>
         <v>745.27</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <f>AVERAGE(B13:B16)</f>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f>AVERAGE(B20:B23)</f>
         <v>738.70337499999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f>AVERAGE(T2:T5)</f>
+        <v>738.71232888202155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f>330.23/60</f>
+        <v>5.5038333333333336</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f>330.23/70</f>
+        <v>4.7175714285714285</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>